<commit_message>
RRupdated to align with Brown paper methodology
</commit_message>
<xml_diff>
--- a/PIF_PAF/Data/RiskFactorInclusion.xlsx
+++ b/PIF_PAF/Data/RiskFactorInclusion.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/zoey_richards_icr_ac_uk/Documents/Git/UK-cancer-trends/PIF_PAF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="878" documentId="8_{2BAECF65-8E05-4226-937D-D5496033051D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4069A4D1-3D5D-4871-855D-56D4730E3D4C}"/>
+  <xr:revisionPtr revIDLastSave="947" documentId="8_{2BAECF65-8E05-4226-937D-D5496033051D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2CCAC79-1DA9-49AE-92DA-82206A2E6307}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="15840" tabRatio="427" activeTab="3" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
+    <workbookView xWindow="30600" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="427" activeTab="2" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
   </bookViews>
   <sheets>
-    <sheet name="RiskFactors " sheetId="1" r:id="rId1"/>
-    <sheet name="DifferentbyAge" sheetId="5" r:id="rId2"/>
-    <sheet name="RR&lt;50" sheetId="2" r:id="rId3"/>
-    <sheet name="RR&lt;50revised" sheetId="6" r:id="rId4"/>
-    <sheet name="RR&gt;50" sheetId="3" r:id="rId5"/>
-    <sheet name="Potential Risk Factors" sheetId="4" r:id="rId6"/>
+    <sheet name="RR&lt;50revised" sheetId="6" r:id="rId1"/>
+    <sheet name="RR&gt;50revised" sheetId="7" r:id="rId2"/>
+    <sheet name="RiskFactors_CausalEvid" sheetId="1" r:id="rId3"/>
+    <sheet name="DifferentbyAge" sheetId="5" r:id="rId4"/>
+    <sheet name="Potential Risk Factors" sheetId="4" r:id="rId5"/>
+    <sheet name="RR&lt;50_OLD" sheetId="2" r:id="rId6"/>
+    <sheet name="RR&gt;50_OLD" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="215">
   <si>
     <t>Cancer sites</t>
   </si>
@@ -644,13 +645,55 @@
   </si>
   <si>
     <t>1.10 (1.03, 1.18)</t>
+  </si>
+  <si>
+    <t>1.12 (1.07, 1.18)</t>
+  </si>
+  <si>
+    <t>1.21 (1.08, 1.35)</t>
+  </si>
+  <si>
+    <t>1.34 (1.20, 1.48)</t>
+  </si>
+  <si>
+    <t>2.54 (2.27, 2.81)</t>
+  </si>
+  <si>
+    <t>1.01 (0.92, 1.12)</t>
+  </si>
+  <si>
+    <t>1.22 (1.09, 1.37)</t>
+  </si>
+  <si>
+    <t>1.54 (1.25, 1.89)</t>
+  </si>
+  <si>
+    <t>1.75 (1.44, 2.14)</t>
+  </si>
+  <si>
+    <t>1.09 (1.02, 1.16)</t>
+  </si>
+  <si>
+    <t>1.15 (1.03, 1.29)</t>
+  </si>
+  <si>
+    <t>1.45 (1.21, 1.75)</t>
+  </si>
+  <si>
+    <t>1.28 (1.07, 1.54)</t>
+  </si>
+  <si>
+    <t>1.10 (1.06, 1.13)</t>
+  </si>
+  <si>
+    <t>1.18 (1.12, 1.25)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -696,13 +739,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1200,7 +1236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1412,12 +1448,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1427,48 +1457,27 @@
     <xf numFmtId="2" fontId="5" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="7" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="7" fillId="3" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="4" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1481,13 +1490,34 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="20" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="6" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="27" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="11" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1506,6 +1536,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1824,14 +1858,1017 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76266A31-B2DD-4192-A61F-66D7D39FE808}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F39" sqref="F39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
+    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
+    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="83"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="96"/>
+      <c r="L3" s="89" t="s">
+        <v>204</v>
+      </c>
+      <c r="M3" s="84"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="89" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="89" t="s">
+        <v>211</v>
+      </c>
+      <c r="L4" s="89" t="s">
+        <v>212</v>
+      </c>
+      <c r="M4" s="84"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="86"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="60"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="89" t="s">
+        <v>205</v>
+      </c>
+      <c r="J5" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="89" t="s">
+        <v>207</v>
+      </c>
+      <c r="L5" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="M5" s="84"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="86"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="95" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="95" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" s="98" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="95" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="89" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="H7" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="J7" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="K7" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="L7" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="M7" s="84"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="86"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="89" t="s">
+        <v>193</v>
+      </c>
+      <c r="J8" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="89" t="s">
+        <v>195</v>
+      </c>
+      <c r="L8" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="M8" s="84"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="86"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="J9" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="K9" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="M9" s="84"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="86"/>
+    </row>
+    <row r="10" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="J10" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="K10" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="L10" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" s="84"/>
+      <c r="N10" s="85"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="86"/>
+    </row>
+    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="101" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="101" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="87"/>
+      <c r="K11" s="87"/>
+      <c r="L11" s="87"/>
+      <c r="M11" s="87"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="104" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="N12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="O12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="47"/>
+      <c r="I14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="92" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="93" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4:H4" r:id="rId1" display="https://pmc.ncbi.nlm.nih.gov/articles/PMC3387822/" xr:uid="{EAAEB933-E6CB-401B-BC9C-DDF1BA2C4BAF}"/>
+    <hyperlink ref="E7:H7" r:id="rId2" display="1.61 (1.38, 1.89)" xr:uid="{087D63A8-8673-4FED-B4AA-78355EFD0EAC}"/>
+    <hyperlink ref="E2:H2" r:id="rId3" display="3.42(2.37, 4.94)" xr:uid="{65242B69-0DF5-4CFB-B061-87593AF2D7D6}"/>
+    <hyperlink ref="E6:F6" r:id="rId4" display="1.14(1.10, 1.18)" xr:uid="{0AC82558-76D8-4A46-86CD-5715FEFF04A8}"/>
+    <hyperlink ref="G6:H6" r:id="rId5" display="1.14(1.10, 1.18)" xr:uid="{357E3F28-1993-4C05-B534-54AE92750BFE}"/>
+    <hyperlink ref="I8:L8" r:id="rId6" display="1.22 (1.17, 1.28)" xr:uid="{C6FBFCCC-6B18-467F-8641-01ACD17463C9}"/>
+    <hyperlink ref="I7:L7" r:id="rId7" display="1.18 (1.06, 1.31)" xr:uid="{C5E12774-A930-4FA2-908D-F9616EB66494}"/>
+    <hyperlink ref="I9:L9" r:id="rId8" display="1.10 (1.03, 1.18)" xr:uid="{A3C6A6BA-ABC5-480C-92FC-62A49715B851}"/>
+    <hyperlink ref="I10:L10" r:id="rId9" display="1.12 (1.07, 1.18)" xr:uid="{BAE65CBC-6E4B-4AA4-B583-22AB3104651C}"/>
+    <hyperlink ref="I3:L3" r:id="rId10" display="https://pubmed.ncbi.nlm.nih.gov/26026348/" xr:uid="{255D8DE5-2107-481F-890F-EA2766EE6B49}"/>
+    <hyperlink ref="I6:L6" r:id="rId11" location="sec13" display="1.22(1.10, 1.36)" xr:uid="{D11D85F1-696C-46A5-9467-2367C9E3106E}"/>
+    <hyperlink ref="M6:O6" r:id="rId12" display="1.18 (1.10, 1.28)" xr:uid="{5F6D7853-A74B-4815-8147-2751460FADAD}"/>
+    <hyperlink ref="P6" r:id="rId13" xr:uid="{D15ADC47-A92A-4580-837C-5FFB47A655C8}"/>
+    <hyperlink ref="Q6" r:id="rId14" xr:uid="{9AE18721-A9FB-47DB-86F2-805C3DBFBB29}"/>
+    <hyperlink ref="I5:L5" r:id="rId15" display="1.01 (0.92, 1.12)" xr:uid="{B1375934-87C9-4618-A990-C5A10D987D42}"/>
+    <hyperlink ref="B2:D2" r:id="rId16" location="sec10" display="1.13(1.00, 1.26)" xr:uid="{02577497-1FFF-4721-BB88-67E7C8483FEC}"/>
+    <hyperlink ref="B6:D7" r:id="rId17" location="sec10" display="0.99 (0.95, 1.04)" xr:uid="{223F5910-7C9F-4125-92C2-315C39551190}"/>
+    <hyperlink ref="B11:D11" r:id="rId18" location="sec10" display="1.04 (1.01, 1.07)" xr:uid="{BF6EF940-63BA-4551-BF0D-43B13E59C027}"/>
+    <hyperlink ref="I4:L4" r:id="rId19" display="1.09 (1.02, 1.16)" xr:uid="{4C515288-CAF1-4FC9-92C6-22CC56393AA9}"/>
+    <hyperlink ref="Q11" r:id="rId20" xr:uid="{BA1C939E-1C5F-49DE-88F3-1DB70A5A2513}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E34ADE-CF51-4185-BC0D-591DEA3B8782}">
+  <dimension ref="A1:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q2" sqref="B2:Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
+    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
+    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="54" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="54" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="J1" s="54" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="L1" s="54" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" s="54" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="P1" s="54" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q1" s="55" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="64" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="94" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="94" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="94" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" s="94" t="s">
+        <v>91</v>
+      </c>
+      <c r="I2" s="91"/>
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="81"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="81"/>
+      <c r="Q2" s="83"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="60"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="84"/>
+      <c r="F3" s="84"/>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="89" t="s">
+        <v>203</v>
+      </c>
+      <c r="K3" s="96"/>
+      <c r="L3" s="89" t="s">
+        <v>204</v>
+      </c>
+      <c r="M3" s="84"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="84"/>
+      <c r="Q3" s="84"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="65" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="60"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
+      <c r="E4" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="F4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="90" t="s">
+        <v>190</v>
+      </c>
+      <c r="H4" s="90" t="s">
+        <v>131</v>
+      </c>
+      <c r="I4" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="J4" s="89" t="s">
+        <v>210</v>
+      </c>
+      <c r="K4" s="89" t="s">
+        <v>211</v>
+      </c>
+      <c r="L4" s="89" t="s">
+        <v>212</v>
+      </c>
+      <c r="M4" s="84"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="85"/>
+      <c r="P4" s="84"/>
+      <c r="Q4" s="86"/>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="65" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="60"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="89" t="s">
+        <v>205</v>
+      </c>
+      <c r="J5" s="89" t="s">
+        <v>206</v>
+      </c>
+      <c r="K5" s="89" t="s">
+        <v>207</v>
+      </c>
+      <c r="L5" s="89" t="s">
+        <v>208</v>
+      </c>
+      <c r="M5" s="84"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="86"/>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="95" t="s">
+        <v>111</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="L6" s="95" t="s">
+        <v>115</v>
+      </c>
+      <c r="M6" s="95" t="s">
+        <v>116</v>
+      </c>
+      <c r="N6" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="O6" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="P6" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q6" s="98" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="97" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="95" t="s">
+        <v>126</v>
+      </c>
+      <c r="E7" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="F7" s="89" t="s">
+        <v>187</v>
+      </c>
+      <c r="G7" s="89" t="s">
+        <v>188</v>
+      </c>
+      <c r="H7" s="89" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="J7" s="89" t="s">
+        <v>197</v>
+      </c>
+      <c r="K7" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="L7" s="89" t="s">
+        <v>198</v>
+      </c>
+      <c r="M7" s="84"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="85"/>
+      <c r="P7" s="84"/>
+      <c r="Q7" s="86"/>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="60"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="84"/>
+      <c r="I8" s="89" t="s">
+        <v>193</v>
+      </c>
+      <c r="J8" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="K8" s="89" t="s">
+        <v>195</v>
+      </c>
+      <c r="L8" s="89" t="s">
+        <v>196</v>
+      </c>
+      <c r="M8" s="84"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="85"/>
+      <c r="P8" s="84"/>
+      <c r="Q8" s="86"/>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="60"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="J9" s="89" t="s">
+        <v>200</v>
+      </c>
+      <c r="K9" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="L9" s="89" t="s">
+        <v>199</v>
+      </c>
+      <c r="M9" s="84"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="84"/>
+      <c r="Q9" s="86"/>
+    </row>
+    <row r="10" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="60"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="84"/>
+      <c r="G10" s="84"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="J10" s="89" t="s">
+        <v>201</v>
+      </c>
+      <c r="K10" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="L10" s="89" t="s">
+        <v>202</v>
+      </c>
+      <c r="M10" s="84"/>
+      <c r="N10" s="85"/>
+      <c r="O10" s="85"/>
+      <c r="P10" s="84"/>
+      <c r="Q10" s="86"/>
+    </row>
+    <row r="11" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="66" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="100" t="s">
+        <v>142</v>
+      </c>
+      <c r="C11" s="101" t="s">
+        <v>143</v>
+      </c>
+      <c r="D11" s="101" t="s">
+        <v>144</v>
+      </c>
+      <c r="E11" s="87"/>
+      <c r="F11" s="87"/>
+      <c r="G11" s="87"/>
+      <c r="H11" s="87"/>
+      <c r="I11" s="87"/>
+      <c r="J11" s="102" t="s">
+        <v>213</v>
+      </c>
+      <c r="K11" s="103"/>
+      <c r="L11" s="102" t="s">
+        <v>214</v>
+      </c>
+      <c r="M11" s="87"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="88"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="104" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="C12" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="M12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="N12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="O12" s="48" t="s">
+        <v>153</v>
+      </c>
+      <c r="P12" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="38"/>
+      <c r="B14" s="47"/>
+      <c r="I14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="K14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="L14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="92" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="93" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E4:H4" r:id="rId1" display="https://pmc.ncbi.nlm.nih.gov/articles/PMC3387822/" xr:uid="{81F149E9-B3ED-4CBF-984F-F57437257CF0}"/>
+    <hyperlink ref="E7:H7" r:id="rId2" display="1.61 (1.38, 1.89)" xr:uid="{31CC389D-7CCF-449D-9343-79D01D35D114}"/>
+    <hyperlink ref="E2:H2" r:id="rId3" display="3.42(2.37, 4.94)" xr:uid="{2863CE85-5F53-42E2-8342-853BC693380C}"/>
+    <hyperlink ref="E6:F6" r:id="rId4" display="1.14(1.10, 1.18)" xr:uid="{8736F32E-DF37-476C-9210-FF353E21F940}"/>
+    <hyperlink ref="G6:H6" r:id="rId5" display="1.14(1.10, 1.18)" xr:uid="{F6B02342-FB92-4F43-B7DB-C3D251E2F1EA}"/>
+    <hyperlink ref="I8:L8" r:id="rId6" display="1.22 (1.17, 1.28)" xr:uid="{8DFD5543-C7B2-4D84-9FD5-4609400DD12F}"/>
+    <hyperlink ref="I7:L7" r:id="rId7" display="1.18 (1.06, 1.31)" xr:uid="{5A9E96EB-7C9B-4BF0-B4C3-CCF1FD2AC14B}"/>
+    <hyperlink ref="I9:L9" r:id="rId8" display="1.10 (1.03, 1.18)" xr:uid="{BA2F2326-5508-4758-BF88-D59C5A6E4071}"/>
+    <hyperlink ref="I10:L10" r:id="rId9" display="1.12 (1.07, 1.18)" xr:uid="{D934DE68-0203-496B-AFE5-F9CF7915F369}"/>
+    <hyperlink ref="I6:L6" r:id="rId10" location="sec13" display="1.22(1.10, 1.36)" xr:uid="{394B87F3-84D1-4D38-A1C8-E7009D9B27BF}"/>
+    <hyperlink ref="M6:O6" r:id="rId11" display="1.18 (1.10, 1.28)" xr:uid="{80B142BA-7135-48CD-87C1-93761C6AAFE3}"/>
+    <hyperlink ref="P6" r:id="rId12" xr:uid="{037985BE-96D7-40F6-AFA8-F24BB8E62998}"/>
+    <hyperlink ref="Q6" r:id="rId13" xr:uid="{86535937-B9F8-40E9-AA7B-326B68348B00}"/>
+    <hyperlink ref="B2:D2" r:id="rId14" location="sec10" display="1.13(1.00, 1.26)" xr:uid="{77A85752-944D-4AF2-B68E-625728C05AE0}"/>
+    <hyperlink ref="B6:D7" r:id="rId15" location="sec10" display="0.99 (0.95, 1.04)" xr:uid="{A61C2D43-5C2A-45D1-BAD3-39960A7E7DA3}"/>
+    <hyperlink ref="B11:D11" r:id="rId16" location="sec10" display="1.04 (1.01, 1.07)" xr:uid="{35481281-63D9-4639-BC5B-E330C2FF25F6}"/>
+    <hyperlink ref="I3:L3" r:id="rId17" display="https://pubmed.ncbi.nlm.nih.gov/26026348/" xr:uid="{DAF8F591-400B-442E-86AE-93BB8CB15CD8}"/>
+    <hyperlink ref="I5:L5" r:id="rId18" display="1.01 (0.92, 1.12)" xr:uid="{B1514570-EBD5-4145-AC59-A8A3D814EC05}"/>
+    <hyperlink ref="I4:L4" r:id="rId19" display="1.09 (1.02, 1.16)" xr:uid="{B2AD435A-7BF4-4BE7-9D09-ADEFA67CF3A2}"/>
+    <hyperlink ref="J11:L11" r:id="rId20" display="1.10 (1.06, 1.13)" xr:uid="{FB51944E-A5F0-47E9-AD12-FADF6B2EFD86}"/>
+    <hyperlink ref="Q11" r:id="rId21" xr:uid="{0436E71F-D0D9-4E22-AEBC-D7518DB54E4C}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9EA320F-06FF-4FEA-86ED-7AC19E5498BB}">
   <dimension ref="A1:AR20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10:I17"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2928,7 +3965,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A96C4FED-520A-4502-BAD0-D9B36A30D69D}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -3183,15 +4220,143 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFA3E62-B5E1-46B7-BE44-9E016BC6F18E}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.28515625" style="48" customWidth="1"/>
+    <col min="2" max="2" width="13" style="48" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="74" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="48" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="C3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E3" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E4" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="48" t="s">
+        <v>174</v>
+      </c>
+      <c r="C5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="48" t="s">
+        <v>175</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>171</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="48" t="s">
+        <v>181</v>
+      </c>
+      <c r="C9" t="s">
+        <v>171</v>
+      </c>
+      <c r="E9" s="75" t="s">
+        <v>172</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" location=":~:text=Urban%20background%20NO2%20pollution%20has,9%20per%20cent%20since%202022." xr:uid="{AACAB583-CD54-4B7F-855C-333FB3589C88}"/>
+    <hyperlink ref="E4" r:id="rId2" xr:uid="{967B7303-F5DB-4D6D-B5B1-6C6CE0A2921B}"/>
+    <hyperlink ref="E5" r:id="rId3" xr:uid="{0BFF3797-EB59-48C2-B684-936DB0929E6A}"/>
+    <hyperlink ref="E6" r:id="rId4" location=":~:text=Urban%20background%20O3%20pollution%20has,per%20cent%20compared%20to%202022." xr:uid="{53D13016-876E-489E-A7A3-040D2F020214}"/>
+    <hyperlink ref="E7" r:id="rId5" location=":~:text=Between%202013%20and%202019%2C%20the,average%20among%20the%20comparator%20countries." xr:uid="{D8C06D14-BF1D-45E0-B997-1C4A4E869EE2}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{2B5A46F5-F583-4F68-9169-524B25A500F0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23675DB8-6EF1-4CEF-94E0-AE4C6C040B3D}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11:R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3727,446 +4892,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76266A31-B2DD-4192-A61F-66D7D39FE808}">
-  <dimension ref="A1:Q19"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I5" sqref="I5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
-    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="C1" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="D1" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="54" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="54" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="54" t="s">
-        <v>73</v>
-      </c>
-      <c r="H1" s="54" t="s">
-        <v>74</v>
-      </c>
-      <c r="I1" s="54" t="s">
-        <v>75</v>
-      </c>
-      <c r="J1" s="54" t="s">
-        <v>76</v>
-      </c>
-      <c r="K1" s="54" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="54" t="s">
-        <v>78</v>
-      </c>
-      <c r="M1" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="N1" s="54" t="s">
-        <v>80</v>
-      </c>
-      <c r="O1" s="54" t="s">
-        <v>81</v>
-      </c>
-      <c r="P1" s="54" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="55" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="F2" s="103" t="s">
-        <v>91</v>
-      </c>
-      <c r="G2" s="103" t="s">
-        <v>90</v>
-      </c>
-      <c r="H2" s="103" t="s">
-        <v>91</v>
-      </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="84"/>
-      <c r="O2" s="84"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="85"/>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="86"/>
-      <c r="C3" s="87"/>
-      <c r="D3" s="87"/>
-      <c r="E3" s="87"/>
-      <c r="F3" s="87"/>
-      <c r="G3" s="87"/>
-      <c r="H3" s="87"/>
-      <c r="I3" s="87"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="87"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="87"/>
-      <c r="N3" s="89"/>
-      <c r="O3" s="89"/>
-      <c r="P3" s="87"/>
-      <c r="Q3" s="87"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="86"/>
-      <c r="C4" s="87"/>
-      <c r="D4" s="87"/>
-      <c r="E4" s="99" t="s">
-        <v>190</v>
-      </c>
-      <c r="F4" s="99" t="s">
-        <v>131</v>
-      </c>
-      <c r="G4" s="99" t="s">
-        <v>190</v>
-      </c>
-      <c r="H4" s="99" t="s">
-        <v>131</v>
-      </c>
-      <c r="I4" s="88">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="J4" s="88">
-        <v>1.1200000000000001</v>
-      </c>
-      <c r="K4" s="88">
-        <v>1.2</v>
-      </c>
-      <c r="L4" s="88">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="M4" s="87"/>
-      <c r="N4" s="89"/>
-      <c r="O4" s="89"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="90"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="87"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="87"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="88">
-        <v>1</v>
-      </c>
-      <c r="J5" s="88">
-        <v>1.22</v>
-      </c>
-      <c r="K5" s="88">
-        <v>1.54</v>
-      </c>
-      <c r="L5" s="88">
-        <v>1.75</v>
-      </c>
-      <c r="M5" s="87"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="87"/>
-      <c r="Q5" s="90"/>
-    </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="B6" s="91"/>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="105" t="s">
-        <v>110</v>
-      </c>
-      <c r="F6" s="105" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="105" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" s="105" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" s="104"/>
-      <c r="J6" s="104"/>
-      <c r="K6" s="104"/>
-      <c r="L6" s="104"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="88"/>
-      <c r="O6" s="88"/>
-      <c r="P6" s="88"/>
-      <c r="Q6" s="92"/>
-    </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="B7" s="91"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="98" t="s">
-        <v>186</v>
-      </c>
-      <c r="F7" s="98" t="s">
-        <v>187</v>
-      </c>
-      <c r="G7" s="98" t="s">
-        <v>188</v>
-      </c>
-      <c r="H7" s="98" t="s">
-        <v>189</v>
-      </c>
-      <c r="I7" s="98" t="s">
-        <v>197</v>
-      </c>
-      <c r="J7" s="98" t="s">
-        <v>197</v>
-      </c>
-      <c r="K7" s="98" t="s">
-        <v>198</v>
-      </c>
-      <c r="L7" s="98" t="s">
-        <v>198</v>
-      </c>
-      <c r="M7" s="87"/>
-      <c r="N7" s="89"/>
-      <c r="O7" s="89"/>
-      <c r="P7" s="87"/>
-      <c r="Q7" s="90"/>
-    </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="86"/>
-      <c r="C8" s="87"/>
-      <c r="D8" s="87"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="87"/>
-      <c r="G8" s="87"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="98" t="s">
-        <v>193</v>
-      </c>
-      <c r="J8" s="98" t="s">
-        <v>194</v>
-      </c>
-      <c r="K8" s="98" t="s">
-        <v>195</v>
-      </c>
-      <c r="L8" s="98" t="s">
-        <v>196</v>
-      </c>
-      <c r="M8" s="87"/>
-      <c r="N8" s="89"/>
-      <c r="O8" s="89"/>
-      <c r="P8" s="87"/>
-      <c r="Q8" s="90"/>
-    </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="87"/>
-      <c r="D9" s="87"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="87"/>
-      <c r="G9" s="87"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="98" t="s">
-        <v>200</v>
-      </c>
-      <c r="J9" s="98" t="s">
-        <v>200</v>
-      </c>
-      <c r="K9" s="98" t="s">
-        <v>199</v>
-      </c>
-      <c r="L9" s="98" t="s">
-        <v>199</v>
-      </c>
-      <c r="M9" s="87"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="87"/>
-      <c r="Q9" s="90"/>
-    </row>
-    <row r="10" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="87"/>
-      <c r="D10" s="87"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="87"/>
-      <c r="G10" s="87"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="87"/>
-      <c r="N10" s="89"/>
-      <c r="O10" s="89"/>
-      <c r="P10" s="87"/>
-      <c r="Q10" s="90"/>
-    </row>
-    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
-        <v>141</v>
-      </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="95"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="95"/>
-      <c r="N11" s="96"/>
-      <c r="O11" s="96"/>
-      <c r="P11" s="95"/>
-      <c r="Q11" s="97"/>
-    </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="39" t="s">
-        <v>149</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="73" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="73" t="s">
-        <v>152</v>
-      </c>
-      <c r="M12" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="N12" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="O12" s="48" t="s">
-        <v>153</v>
-      </c>
-      <c r="P12" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="Q13"/>
-    </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="47"/>
-      <c r="I14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="J14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q14"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="101" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="102" t="s">
-        <v>192</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E4:H4" r:id="rId1" display="https://pmc.ncbi.nlm.nih.gov/articles/PMC3387822/" xr:uid="{EAAEB933-E6CB-401B-BC9C-DDF1BA2C4BAF}"/>
-    <hyperlink ref="E7:H7" r:id="rId2" display="1.61 (1.38, 1.89)" xr:uid="{087D63A8-8673-4FED-B4AA-78355EFD0EAC}"/>
-    <hyperlink ref="E2:H2" r:id="rId3" display="3.42(2.37, 4.94)" xr:uid="{65242B69-0DF5-4CFB-B061-87593AF2D7D6}"/>
-    <hyperlink ref="E6:F6" r:id="rId4" display="1.14(1.10, 1.18)" xr:uid="{0AC82558-76D8-4A46-86CD-5715FEFF04A8}"/>
-    <hyperlink ref="G6:H6" r:id="rId5" display="1.14(1.10, 1.18)" xr:uid="{357E3F28-1993-4C05-B534-54AE92750BFE}"/>
-    <hyperlink ref="I8:L8" r:id="rId6" display="1.22 (1.17, 1.28)" xr:uid="{C6FBFCCC-6B18-467F-8641-01ACD17463C9}"/>
-    <hyperlink ref="I7:L7" r:id="rId7" display="1.18 (1.06, 1.31)" xr:uid="{C5E12774-A930-4FA2-908D-F9616EB66494}"/>
-    <hyperlink ref="I9:L9" r:id="rId8" display="1.10 (1.03, 1.18)" xr:uid="{A3C6A6BA-ABC5-480C-92FC-62A49715B851}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B81CF4DB-DDEE-4C40-B64F-6299D2FB2094}">
   <dimension ref="A1:V12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4732,155 +5466,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBFA3E62-B5E1-46B7-BE44-9E016BC6F18E}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.28515625" style="48" customWidth="1"/>
-    <col min="2" max="2" width="13" style="48" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
-        <v>164</v>
-      </c>
-      <c r="B1" s="74" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="74" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" s="74" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="48" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="48" t="s">
-        <v>174</v>
-      </c>
-      <c r="C5" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C6" t="s">
-        <v>176</v>
-      </c>
-      <c r="E6" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
-        <v>177</v>
-      </c>
-      <c r="C7" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="48" t="s">
-        <v>178</v>
-      </c>
-      <c r="C8" t="s">
-        <v>179</v>
-      </c>
-      <c r="E8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="48" t="s">
-        <v>181</v>
-      </c>
-      <c r="C9" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9" s="75" t="s">
-        <v>172</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" location=":~:text=Urban%20background%20NO2%20pollution%20has,9%20per%20cent%20since%202022." xr:uid="{AACAB583-CD54-4B7F-855C-333FB3589C88}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{967B7303-F5DB-4D6D-B5B1-6C6CE0A2921B}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{0BFF3797-EB59-48C2-B684-936DB0929E6A}"/>
-    <hyperlink ref="E6" r:id="rId4" location=":~:text=Urban%20background%20O3%20pollution%20has,per%20cent%20compared%20to%202022." xr:uid="{53D13016-876E-489E-A7A3-040D2F020214}"/>
-    <hyperlink ref="E7" r:id="rId5" location=":~:text=Between%202013%20and%202019%2C%20the,average%20among%20the%20comparator%20countries." xr:uid="{D8C06D14-BF1D-45E0-B997-1C4A4E869EE2}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{2B5A46F5-F583-4F68-9169-524B25A500F0}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd2fdf2a-32c1-407b-9ced-add881464c8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffa11740-9928-41bb-ae58-1a516ad56a77">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F23E56906CF48E4898EBBEC32E886C77" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40cb373ebc45d73d7e98756bdb2f8cfa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffa11740-9928-41bb-ae58-1a516ad56a77" xmlns:ns3="dd2fdf2a-32c1-407b-9ced-add881464c8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9902785ce56e669554ee78f7e0db075b" ns2:_="" ns3:_="">
     <xsd:import namespace="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
@@ -5075,10 +5661,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd2fdf2a-32c1-407b-9ced-add881464c8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffa11740-9928-41bb-ae58-1a516ad56a77">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82557EFD-ABDD-4D48-A2CB-18202A56A835}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D5640F-C837-4E39-9EE0-62E8F506E068}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
+    <ds:schemaRef ds:uri="dd2fdf2a-32c1-407b-9ced-add881464c8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5101,20 +5718,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D5640F-C837-4E39-9EE0-62E8F506E068}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82557EFD-ABDD-4D48-A2CB-18202A56A835}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
-    <ds:schemaRef ds:uri="dd2fdf2a-32c1-407b-9ced-add881464c8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
PA and endometrial cancer RR added
</commit_message>
<xml_diff>
--- a/PIF_PAF/Data/RiskFactorInclusion.xlsx
+++ b/PIF_PAF/Data/RiskFactorInclusion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/zoey_richards_icr_ac_uk/Documents/Git/UK-cancer-trends/PIF_PAF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="114_{09FAF919-D4F1-4CA3-ACE3-7A26F36E97CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="114_{09FAF919-D4F1-4CA3-ACE3-7A26F36E97CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27830B17-014A-439A-9EF8-8DE80AB32C31}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="15840" tabRatio="427" activeTab="1" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="427" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
   </bookViews>
   <sheets>
     <sheet name="RR&lt;50revised" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="215">
   <si>
     <t>Cancer sites</t>
   </si>
@@ -1236,7 +1236,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1518,6 +1518,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1857,24 +1860,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76266A31-B2DD-4192-A61F-66D7D39FE808}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
-    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="4" width="18.54296875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" style="37" customWidth="1"/>
+    <col min="8" max="11" width="18.54296875" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" style="37" customWidth="1"/>
+    <col min="13" max="17" width="18.54296875" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="63" t="s">
         <v>67</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="64" t="s">
         <v>43</v>
       </c>
@@ -1962,7 +1965,7 @@
       <c r="P2" s="81"/>
       <c r="Q2" s="83"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>47</v>
       </c>
@@ -1985,9 +1988,11 @@
       <c r="N3" s="85"/>
       <c r="O3" s="85"/>
       <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>48</v>
       </c>
@@ -2024,7 +2029,7 @@
       <c r="P4" s="84"/>
       <c r="Q4" s="86"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>49</v>
       </c>
@@ -2053,7 +2058,7 @@
       <c r="P5" s="84"/>
       <c r="Q5" s="86"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
@@ -2106,7 +2111,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>51</v>
       </c>
@@ -2149,7 +2154,7 @@
       <c r="P7" s="84"/>
       <c r="Q7" s="86"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>52</v>
       </c>
@@ -2178,7 +2183,7 @@
       <c r="P8" s="84"/>
       <c r="Q8" s="86"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>53</v>
       </c>
@@ -2207,7 +2212,7 @@
       <c r="P9" s="84"/>
       <c r="Q9" s="86"/>
     </row>
-    <row r="10" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>54</v>
       </c>
@@ -2236,7 +2241,7 @@
       <c r="P10" s="84"/>
       <c r="Q10" s="86"/>
     </row>
-    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="66" t="s">
         <v>141</v>
       </c>
@@ -2265,7 +2270,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>149</v>
       </c>
@@ -2294,10 +2299,10 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q13"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="47"/>
       <c r="I14" s="37" t="s">
@@ -2314,12 +2319,12 @@
       </c>
       <c r="Q14"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="92" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="93" t="s">
         <v>191</v>
       </c>
@@ -2346,9 +2351,10 @@
     <hyperlink ref="B11:D11" r:id="rId18" location="sec10" display="1.04 (1.01, 1.07)" xr:uid="{BF6EF940-63BA-4551-BF0D-43B13E59C027}"/>
     <hyperlink ref="I4:L4" r:id="rId19" display="1.09 (1.02, 1.16)" xr:uid="{4C515288-CAF1-4FC9-92C6-22CC56393AA9}"/>
     <hyperlink ref="Q11" r:id="rId20" xr:uid="{BA1C939E-1C5F-49DE-88F3-1DB70A5A2513}"/>
+    <hyperlink ref="Q3" r:id="rId21" location="full-view-affiliation-1" xr:uid="{D693F8E4-BF53-45A6-B723-FFEF11CFAC89}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
@@ -2356,24 +2362,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E34ADE-CF51-4185-BC0D-591DEA3B8782}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
-    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="4" width="18.54296875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" style="37" customWidth="1"/>
+    <col min="8" max="11" width="18.54296875" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" style="37" customWidth="1"/>
+    <col min="13" max="17" width="18.54296875" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="63" t="s">
         <v>67</v>
       </c>
@@ -2426,7 +2432,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="64" t="s">
         <v>43</v>
       </c>
@@ -2461,7 +2467,7 @@
       <c r="P2" s="81"/>
       <c r="Q2" s="83"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>47</v>
       </c>
@@ -2484,9 +2490,11 @@
       <c r="N3" s="85"/>
       <c r="O3" s="85"/>
       <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-    </row>
-    <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="105" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>48</v>
       </c>
@@ -2523,7 +2531,7 @@
       <c r="P4" s="84"/>
       <c r="Q4" s="86"/>
     </row>
-    <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>49</v>
       </c>
@@ -2552,7 +2560,7 @@
       <c r="P5" s="84"/>
       <c r="Q5" s="86"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
@@ -2605,7 +2613,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>51</v>
       </c>
@@ -2648,7 +2656,7 @@
       <c r="P7" s="84"/>
       <c r="Q7" s="86"/>
     </row>
-    <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>52</v>
       </c>
@@ -2677,7 +2685,7 @@
       <c r="P8" s="84"/>
       <c r="Q8" s="86"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>53</v>
       </c>
@@ -2706,7 +2714,7 @@
       <c r="P9" s="84"/>
       <c r="Q9" s="86"/>
     </row>
-    <row r="10" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>54</v>
       </c>
@@ -2735,7 +2743,7 @@
       <c r="P10" s="84"/>
       <c r="Q10" s="86"/>
     </row>
-    <row r="11" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="66" t="s">
         <v>141</v>
       </c>
@@ -2768,7 +2776,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>149</v>
       </c>
@@ -2797,10 +2805,10 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="Q13"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="47"/>
       <c r="I14" s="37" t="s">
@@ -2817,12 +2825,12 @@
       </c>
       <c r="Q14"/>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="92" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="93" t="s">
         <v>191</v>
       </c>
@@ -2850,9 +2858,10 @@
     <hyperlink ref="I4:L4" r:id="rId19" display="1.09 (1.02, 1.16)" xr:uid="{B2AD435A-7BF4-4BE7-9D09-ADEFA67CF3A2}"/>
     <hyperlink ref="J11:L11" r:id="rId20" display="1.10 (1.06, 1.13)" xr:uid="{FB51944E-A5F0-47E9-AD12-FADF6B2EFD86}"/>
     <hyperlink ref="Q11" r:id="rId21" xr:uid="{0436E71F-D0D9-4E22-AEBC-D7518DB54E4C}"/>
+    <hyperlink ref="Q3" r:id="rId22" location="full-view-affiliation-1" xr:uid="{0C6124C5-70A8-40F6-85E8-CB17A0954AAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2867,17 +2876,17 @@
       <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="4" width="11.140625" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="7"/>
-    <col min="7" max="8" width="11.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.1796875" customWidth="1"/>
+    <col min="2" max="4" width="11.1796875" customWidth="1"/>
+    <col min="5" max="5" width="12.7265625" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="7"/>
+    <col min="7" max="8" width="11.1796875" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="1" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="1" customFormat="1" ht="71.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -3011,7 +3020,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>43</v>
       </c>
@@ -3069,7 +3078,7 @@
       <c r="AQ2" s="5"/>
       <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
@@ -3131,7 +3140,7 @@
       <c r="AQ3" s="5"/>
       <c r="AR3" s="5"/>
     </row>
-    <row r="4" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>48</v>
       </c>
@@ -3187,7 +3196,7 @@
       <c r="AQ4" s="5"/>
       <c r="AR4" s="5"/>
     </row>
-    <row r="5" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
@@ -3239,7 +3248,7 @@
       <c r="AQ5" s="5"/>
       <c r="AR5" s="5"/>
     </row>
-    <row r="6" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
@@ -3311,7 +3320,7 @@
       <c r="AQ6" s="5"/>
       <c r="AR6" s="5"/>
     </row>
-    <row r="7" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
@@ -3381,7 +3390,7 @@
       <c r="AQ7" s="5"/>
       <c r="AR7" s="5"/>
     </row>
-    <row r="8" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
@@ -3437,7 +3446,7 @@
       <c r="AQ8" s="5"/>
       <c r="AR8" s="5"/>
     </row>
-    <row r="9" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -3491,7 +3500,7 @@
       <c r="AQ9" s="5"/>
       <c r="AR9" s="5"/>
     </row>
-    <row r="10" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>54</v>
       </c>
@@ -3545,7 +3554,7 @@
       <c r="AQ10" s="5"/>
       <c r="AR10" s="5"/>
     </row>
-    <row r="11" spans="1:44" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="35" t="s">
         <v>55</v>
       </c>
@@ -3615,7 +3624,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>56</v>
       </c>
@@ -3675,7 +3684,7 @@
       <c r="AQ12" s="5"/>
       <c r="AR12" s="5"/>
     </row>
-    <row r="13" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>58</v>
       </c>
@@ -3727,7 +3736,7 @@
       <c r="AQ13" s="5"/>
       <c r="AR13" s="5"/>
     </row>
-    <row r="14" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>59</v>
       </c>
@@ -3779,7 +3788,7 @@
       <c r="AQ14" s="5"/>
       <c r="AR14" s="5"/>
     </row>
-    <row r="15" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>60</v>
       </c>
@@ -3829,7 +3838,7 @@
       <c r="AQ15" s="5"/>
       <c r="AR15" s="5"/>
     </row>
-    <row r="16" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" ht="33" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
         <v>61</v>
       </c>
@@ -3885,7 +3894,7 @@
       <c r="AQ16" s="5"/>
       <c r="AR16" s="5"/>
     </row>
-    <row r="17" spans="1:44" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="17" t="s">
         <v>62</v>
       </c>
@@ -3943,12 +3952,12 @@
       <c r="AQ17" s="5"/>
       <c r="AR17" s="5"/>
     </row>
-    <row r="19" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A19" s="67" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>64</v>
       </c>
@@ -3969,13 +3978,13 @@
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="2" max="12" width="11.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="12" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="37" customFormat="1" ht="71.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="37" customFormat="1" ht="70" x14ac:dyDescent="0.35">
       <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
@@ -4013,7 +4022,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>43</v>
       </c>
@@ -4029,7 +4038,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
@@ -4051,7 +4060,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>48</v>
       </c>
@@ -4069,7 +4078,7 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
@@ -4087,7 +4096,7 @@
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
@@ -4119,7 +4128,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
     </row>
-    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
@@ -4137,7 +4146,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
@@ -4153,7 +4162,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -4169,7 +4178,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>54</v>
       </c>
@@ -4185,7 +4194,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>55</v>
       </c>
@@ -4224,15 +4233,15 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="48" customWidth="1"/>
+    <col min="1" max="1" width="15.26953125" style="48" customWidth="1"/>
     <col min="2" max="2" width="13" style="48" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.1796875" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="74" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="74" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="74" t="s">
         <v>164</v>
       </c>
@@ -4249,12 +4258,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="48" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="48" t="s">
         <v>170</v>
       </c>
@@ -4265,7 +4274,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B4" s="48" t="s">
         <v>173</v>
       </c>
@@ -4276,7 +4285,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B5" s="48" t="s">
         <v>174</v>
       </c>
@@ -4287,7 +4296,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B6" s="48" t="s">
         <v>175</v>
       </c>
@@ -4298,7 +4307,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="48" t="s">
         <v>177</v>
       </c>
@@ -4309,7 +4318,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="48" t="s">
         <v>178</v>
       </c>
@@ -4320,7 +4329,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="48" t="s">
         <v>181</v>
       </c>
@@ -4355,21 +4364,21 @@
       <selection pane="bottomRight" activeCell="Q11" sqref="Q11:R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
-    <col min="13" max="18" width="18.5703125" style="37" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
-    <col min="20" max="20" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.26953125" customWidth="1"/>
+    <col min="2" max="4" width="18.54296875" style="37" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="37" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" style="37" customWidth="1"/>
+    <col min="7" max="7" width="19.453125" style="37" customWidth="1"/>
+    <col min="8" max="11" width="18.54296875" style="37" customWidth="1"/>
+    <col min="12" max="12" width="20.26953125" style="37" customWidth="1"/>
+    <col min="13" max="18" width="18.54296875" style="37" customWidth="1"/>
+    <col min="19" max="19" width="16.7265625" customWidth="1"/>
+    <col min="20" max="20" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="56" customFormat="1" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" s="56" customFormat="1" ht="30.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="63" t="s">
         <v>67</v>
       </c>
@@ -4431,7 +4440,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="64" t="s">
         <v>43</v>
       </c>
@@ -4469,7 +4478,7 @@
       <c r="S2" s="53"/>
       <c r="T2" s="53"/>
     </row>
-    <row r="3" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="65" t="s">
         <v>47</v>
       </c>
@@ -4497,7 +4506,7 @@
       <c r="S3" s="53"/>
       <c r="T3" s="53"/>
     </row>
-    <row r="4" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="65" t="s">
         <v>48</v>
       </c>
@@ -4537,7 +4546,7 @@
       <c r="S4" s="53"/>
       <c r="T4" s="53"/>
     </row>
-    <row r="5" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="65" t="s">
         <v>49</v>
       </c>
@@ -4569,7 +4578,7 @@
       <c r="S5" s="53"/>
       <c r="T5" s="53"/>
     </row>
-    <row r="6" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
@@ -4627,7 +4636,7 @@
       <c r="S6" s="53"/>
       <c r="T6" s="53"/>
     </row>
-    <row r="7" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="65" t="s">
         <v>51</v>
       </c>
@@ -4673,7 +4682,7 @@
       <c r="S7" s="53"/>
       <c r="T7" s="53"/>
     </row>
-    <row r="8" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="65" t="s">
         <v>52</v>
       </c>
@@ -4705,7 +4714,7 @@
       <c r="S8" s="43"/>
       <c r="T8" s="43"/>
     </row>
-    <row r="9" spans="1:20" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="65" t="s">
         <v>53</v>
       </c>
@@ -4737,7 +4746,7 @@
       <c r="S9" s="43"/>
       <c r="T9" s="43"/>
     </row>
-    <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="65" t="s">
         <v>54</v>
       </c>
@@ -4769,7 +4778,7 @@
       <c r="S10" s="43"/>
       <c r="T10" s="43"/>
     </row>
-    <row r="11" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="66" t="s">
         <v>141</v>
       </c>
@@ -4803,7 +4812,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>149</v>
       </c>
@@ -4838,10 +4847,10 @@
         <v>159</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="38"/>
       <c r="B14" s="47"/>
       <c r="I14" s="37" t="s">
@@ -4899,21 +4908,21 @@
       <selection pane="bottomRight" activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
-    <col min="13" max="18" width="19.42578125" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="9" width="19.453125" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" customWidth="1"/>
+    <col min="12" max="12" width="21.26953125" customWidth="1"/>
+    <col min="13" max="18" width="19.453125" customWidth="1"/>
+    <col min="19" max="19" width="16.54296875" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="56" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="56" customFormat="1" ht="30" x14ac:dyDescent="0.35">
       <c r="A1" s="63" t="s">
         <v>67</v>
       </c>
@@ -4981,7 +4990,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="49" t="s">
         <v>43</v>
       </c>
@@ -5021,7 +5030,7 @@
       <c r="U2" s="53"/>
       <c r="V2" s="53"/>
     </row>
-    <row r="3" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
         <v>47</v>
       </c>
@@ -5057,7 +5066,7 @@
       <c r="U3" s="53"/>
       <c r="V3" s="53"/>
     </row>
-    <row r="4" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="13" t="s">
         <v>48</v>
       </c>
@@ -5099,7 +5108,7 @@
       <c r="U4" s="53"/>
       <c r="V4" s="53"/>
     </row>
-    <row r="5" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>49</v>
       </c>
@@ -5133,7 +5142,7 @@
       <c r="U5" s="53"/>
       <c r="V5" s="53"/>
     </row>
-    <row r="6" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>50</v>
       </c>
@@ -5197,7 +5206,7 @@
       <c r="U6" s="53"/>
       <c r="V6" s="53"/>
     </row>
-    <row r="7" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
@@ -5245,7 +5254,7 @@
       <c r="U7" s="53"/>
       <c r="V7" s="53"/>
     </row>
-    <row r="8" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>52</v>
       </c>
@@ -5279,7 +5288,7 @@
       <c r="U8" s="43"/>
       <c r="V8" s="43"/>
     </row>
-    <row r="9" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>53</v>
       </c>
@@ -5313,7 +5322,7 @@
       <c r="U9" s="43"/>
       <c r="V9" s="43"/>
     </row>
-    <row r="10" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>54</v>
       </c>
@@ -5347,7 +5356,7 @@
       <c r="U10" s="43"/>
       <c r="V10" s="43"/>
     </row>
-    <row r="11" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="35" t="s">
         <v>55</v>
       </c>
@@ -5391,7 +5400,7 @@
       </c>
       <c r="V11" s="43"/>
     </row>
-    <row r="12" spans="1:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="39" t="s">
         <v>149</v>
       </c>
@@ -5463,6 +5472,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="dd2fdf2a-32c1-407b-9ced-add881464c8a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffa11740-9928-41bb-ae58-1a516ad56a77">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F23E56906CF48E4898EBBEC32E886C77" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="40cb373ebc45d73d7e98756bdb2f8cfa">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ffa11740-9928-41bb-ae58-1a516ad56a77" xmlns:ns3="dd2fdf2a-32c1-407b-9ced-add881464c8a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9902785ce56e669554ee78f7e0db075b" ns2:_="" ns3:_="">
     <xsd:import namespace="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
@@ -5657,41 +5686,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="dd2fdf2a-32c1-407b-9ced-add881464c8a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ffa11740-9928-41bb-ae58-1a516ad56a77">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D5640F-C837-4E39-9EE0-62E8F506E068}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82557EFD-ABDD-4D48-A2CB-18202A56A835}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
-    <ds:schemaRef ds:uri="dd2fdf2a-32c1-407b-9ced-add881464c8a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5714,9 +5712,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82557EFD-ABDD-4D48-A2CB-18202A56A835}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14D5640F-C837-4E39-9EE0-62E8F506E068}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ffa11740-9928-41bb-ae58-1a516ad56a77"/>
+    <ds:schemaRef ds:uri="dd2fdf2a-32c1-407b-9ced-add881464c8a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updating figures on new RRs
</commit_message>
<xml_diff>
--- a/PIF_PAF/Data/RiskFactorInclusion.xlsx
+++ b/PIF_PAF/Data/RiskFactorInclusion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://icracuk-my.sharepoint.com/personal/reuben_frost_icr_ac_uk/Documents/Documents/PAF/UK-cancer-trends/PIF_PAF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="114_{09FAF919-D4F1-4CA3-ACE3-7A26F36E97CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B3194ECB-3FC8-48CB-96D3-0DD5CFB55008}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="114_{09FAF919-D4F1-4CA3-ACE3-7A26F36E97CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C87D633-6173-4822-A14E-C860483D7B3B}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="105" windowWidth="38640" windowHeight="21240" tabRatio="427" activeTab="1" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="427" xr2:uid="{82C8E521-6593-413B-AA3E-36C522030C71}"/>
   </bookViews>
   <sheets>
     <sheet name="RR&lt;50revised" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="246">
   <si>
     <t>Cancer sites</t>
   </si>
@@ -693,6 +693,93 @@
   </si>
   <si>
     <t>0.93 (0.87, 0.99)</t>
+  </si>
+  <si>
+    <t>Light_alcohol_men</t>
+  </si>
+  <si>
+    <t>Medium_alcohol_men</t>
+  </si>
+  <si>
+    <t>Heavy_alcohol_men</t>
+  </si>
+  <si>
+    <t>Light_alcohol_women</t>
+  </si>
+  <si>
+    <t>Medium_alcohol_women</t>
+  </si>
+  <si>
+    <t>Heavy_alcohol_women</t>
+  </si>
+  <si>
+    <t>1.20 (1.06, 1.35)</t>
+  </si>
+  <si>
+    <t>2.01 (1.69, 2.40)</t>
+  </si>
+  <si>
+    <t>5.33 (4.28, 6.63)</t>
+  </si>
+  <si>
+    <t>1.00 (0.78, 1.27)</t>
+  </si>
+  <si>
+    <t>1.67 (1.25, 2.22)</t>
+  </si>
+  <si>
+    <t>5.70 (3.75, 8.66)</t>
+  </si>
+  <si>
+    <t>1.05 (0.95, 1.16)</t>
+  </si>
+  <si>
+    <t>1.21 (1.11, 1.32)</t>
+  </si>
+  <si>
+    <t>1.53 (1.30, 1.80)</t>
+  </si>
+  <si>
+    <t>0.95 (0.89, 1.01)</t>
+  </si>
+  <si>
+    <t>1.07 (0.99, 1.16)</t>
+  </si>
+  <si>
+    <t>1.24 (0.68, 2.25)</t>
+  </si>
+  <si>
+    <t>1.05 (0.84, 1.32)</t>
+  </si>
+  <si>
+    <t>1.08 (0.88, 1.32)</t>
+  </si>
+  <si>
+    <t>1.59 (1.21, 2.09)</t>
+  </si>
+  <si>
+    <t>0.81 (0.59, 1.12)</t>
+  </si>
+  <si>
+    <t>1.24 (0.88, 1.75)</t>
+  </si>
+  <si>
+    <t>3.89 (1.60, 9.48)</t>
+  </si>
+  <si>
+    <t>1.39 (1.28, 1.51)</t>
+  </si>
+  <si>
+    <t>1.20 (1.14, 1.27)</t>
+  </si>
+  <si>
+    <t>1.06 (1.03, 1.10)</t>
+  </si>
+  <si>
+    <t>1.22 (1.17, 1.27)</t>
+  </si>
+  <si>
+    <t>1.50 (1.19, 1.89)</t>
   </si>
 </sst>
 </file>
@@ -1242,7 +1329,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1531,6 +1618,9 @@
     </xf>
     <xf numFmtId="2" fontId="6" fillId="2" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1867,425 +1957,490 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76266A31-B2DD-4192-A61F-66D7D39FE808}">
-  <dimension ref="A1:R19"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R6" sqref="Q6:R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="4" width="18.5703125" style="37" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="37" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="37" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="37" customWidth="1"/>
-    <col min="8" max="11" width="18.5703125" style="37" customWidth="1"/>
-    <col min="12" max="12" width="20.28515625" style="37" customWidth="1"/>
-    <col min="13" max="17" width="18.5703125" style="37" customWidth="1"/>
+    <col min="2" max="7" width="18.5703125" style="37" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" style="37" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="37" customWidth="1"/>
+    <col min="11" max="14" width="18.5703125" style="37" customWidth="1"/>
+    <col min="15" max="15" width="20.28515625" style="37" customWidth="1"/>
+    <col min="16" max="20" width="18.5703125" style="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="63" t="s">
         <v>67</v>
       </c>
       <c r="B1" s="58" t="s">
-        <v>68</v>
+        <v>217</v>
       </c>
       <c r="C1" s="54" t="s">
-        <v>69</v>
+        <v>218</v>
       </c>
       <c r="D1" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="54" t="s">
+        <v>219</v>
+      </c>
+      <c r="E1" s="58" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" s="54" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" s="54" t="s">
+        <v>222</v>
+      </c>
+      <c r="H1" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="F1" s="54" t="s">
+      <c r="I1" s="54" t="s">
         <v>72</v>
       </c>
-      <c r="G1" s="54" t="s">
+      <c r="J1" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H1" s="54" t="s">
+      <c r="K1" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="L1" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="M1" s="54" t="s">
         <v>76</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="N1" s="54" t="s">
         <v>77</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="O1" s="54" t="s">
         <v>78</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="P1" s="54" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="Q1" s="54" t="s">
         <v>80</v>
       </c>
-      <c r="O1" s="54" t="s">
+      <c r="R1" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="P1" s="54" t="s">
+      <c r="S1" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="55" t="s">
+      <c r="T1" s="55" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="64" t="s">
         <v>43</v>
       </c>
       <c r="B2" s="99" t="s">
-        <v>87</v>
+        <v>223</v>
       </c>
       <c r="C2" s="94" t="s">
-        <v>88</v>
+        <v>224</v>
       </c>
       <c r="D2" s="94" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="94" t="s">
+        <v>225</v>
+      </c>
+      <c r="E2" s="99" t="s">
+        <v>226</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>227</v>
+      </c>
+      <c r="G2" s="94" t="s">
+        <v>228</v>
+      </c>
+      <c r="H2" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="F2" s="94" t="s">
+      <c r="I2" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="G2" s="94" t="s">
+      <c r="J2" s="94" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="94" t="s">
+      <c r="K2" s="94" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="91"/>
-      <c r="J2" s="91"/>
-      <c r="K2" s="91"/>
       <c r="L2" s="91"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
       <c r="P2" s="81"/>
-      <c r="Q2" s="83"/>
-    </row>
-    <row r="3" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="83"/>
+    </row>
+    <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="65" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="60"/>
       <c r="C3" s="40"/>
       <c r="D3" s="40"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
       <c r="H3" s="84"/>
-      <c r="I3" s="96"/>
-      <c r="J3" s="89" t="s">
+      <c r="I3" s="84"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="84"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="89" t="s">
         <v>202</v>
       </c>
-      <c r="K3" s="96"/>
-      <c r="L3" s="89" t="s">
+      <c r="N3" s="96"/>
+      <c r="O3" s="89" t="s">
         <v>203</v>
       </c>
-      <c r="M3" s="84"/>
-      <c r="N3" s="85"/>
-      <c r="O3" s="85"/>
       <c r="P3" s="84"/>
-      <c r="Q3" s="105" t="s">
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="84"/>
+      <c r="T3" s="105" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="65" t="s">
         <v>48</v>
       </c>
       <c r="B4" s="60"/>
       <c r="C4" s="40"/>
       <c r="D4" s="40"/>
-      <c r="E4" s="90" t="s">
+      <c r="E4" s="60"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="I4" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="G4" s="90" t="s">
+      <c r="J4" s="90" t="s">
         <v>214</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="K4" s="90" t="s">
         <v>131</v>
       </c>
-      <c r="I4" s="89" t="s">
+      <c r="L4" s="89" t="s">
         <v>208</v>
       </c>
-      <c r="J4" s="89" t="s">
+      <c r="M4" s="89" t="s">
         <v>209</v>
       </c>
-      <c r="K4" s="89" t="s">
+      <c r="N4" s="89" t="s">
         <v>210</v>
       </c>
-      <c r="L4" s="89" t="s">
+      <c r="O4" s="89" t="s">
         <v>211</v>
       </c>
-      <c r="M4" s="84"/>
-      <c r="N4" s="85"/>
-      <c r="O4" s="85"/>
       <c r="P4" s="84"/>
-      <c r="Q4" s="86"/>
-    </row>
-    <row r="5" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q4" s="85"/>
+      <c r="R4" s="85"/>
+      <c r="S4" s="84"/>
+      <c r="T4" s="86"/>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="65" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="40"/>
       <c r="D5" s="40"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
       <c r="H5" s="84"/>
-      <c r="I5" s="89" t="s">
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="89" t="s">
         <v>204</v>
       </c>
-      <c r="J5" s="89" t="s">
+      <c r="M5" s="89" t="s">
         <v>205</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="N5" s="89" t="s">
         <v>206</v>
       </c>
-      <c r="L5" s="89" t="s">
+      <c r="O5" s="89" t="s">
         <v>207</v>
       </c>
-      <c r="M5" s="84"/>
-      <c r="N5" s="85"/>
-      <c r="O5" s="85"/>
       <c r="P5" s="84"/>
-      <c r="Q5" s="86"/>
-    </row>
-    <row r="6" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="86"/>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="65" t="s">
         <v>50</v>
       </c>
       <c r="B6" s="97" t="s">
-        <v>107</v>
+        <v>229</v>
       </c>
       <c r="C6" s="95" t="s">
-        <v>108</v>
+        <v>230</v>
       </c>
       <c r="D6" s="95" t="s">
-        <v>109</v>
-      </c>
-      <c r="E6" s="95" t="s">
+        <v>231</v>
+      </c>
+      <c r="E6" s="97" t="s">
+        <v>232</v>
+      </c>
+      <c r="F6" s="95" t="s">
+        <v>233</v>
+      </c>
+      <c r="G6" s="95" t="s">
+        <v>234</v>
+      </c>
+      <c r="H6" s="95" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="95" t="s">
+      <c r="I6" s="95" t="s">
         <v>111</v>
       </c>
-      <c r="G6" s="95" t="s">
+      <c r="J6" s="95" t="s">
         <v>112</v>
       </c>
-      <c r="H6" s="95" t="s">
+      <c r="K6" s="95" t="s">
         <v>113</v>
       </c>
-      <c r="I6" s="95" t="s">
+      <c r="L6" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="J6" s="95" t="s">
+      <c r="M6" s="95" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="95" t="s">
+      <c r="N6" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="L6" s="95" t="s">
+      <c r="O6" s="95" t="s">
         <v>115</v>
       </c>
-      <c r="M6" s="95" t="s">
+      <c r="P6" s="95" t="s">
         <v>116</v>
       </c>
-      <c r="N6" s="95" t="s">
+      <c r="Q6" s="95" t="s">
         <v>117</v>
       </c>
-      <c r="O6" s="95" t="s">
+      <c r="R6" s="95" t="s">
         <v>118</v>
       </c>
-      <c r="P6" s="95" t="s">
+      <c r="S6" s="95" t="s">
         <v>119</v>
       </c>
-      <c r="Q6" s="98" t="s">
+      <c r="T6" s="98" t="s">
         <v>215</v>
       </c>
-      <c r="R6" s="75"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="U6" s="75"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="65" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="97" t="s">
-        <v>124</v>
+        <v>235</v>
       </c>
       <c r="C7" s="95" t="s">
-        <v>125</v>
+        <v>236</v>
       </c>
       <c r="D7" s="95" t="s">
-        <v>126</v>
-      </c>
-      <c r="E7" s="89" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" s="97" t="s">
+        <v>238</v>
+      </c>
+      <c r="F7" s="95" t="s">
+        <v>239</v>
+      </c>
+      <c r="G7" s="95" t="s">
+        <v>240</v>
+      </c>
+      <c r="H7" s="89" t="s">
         <v>186</v>
       </c>
-      <c r="F7" s="89" t="s">
+      <c r="I7" s="89" t="s">
         <v>187</v>
       </c>
-      <c r="G7" s="89" t="s">
+      <c r="J7" s="89" t="s">
         <v>188</v>
       </c>
-      <c r="H7" s="89" t="s">
+      <c r="K7" s="89" t="s">
         <v>189</v>
       </c>
-      <c r="I7" s="89" t="s">
+      <c r="L7" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="J7" s="89" t="s">
+      <c r="M7" s="89" t="s">
         <v>196</v>
       </c>
-      <c r="K7" s="89" t="s">
+      <c r="N7" s="89" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="89" t="s">
+      <c r="O7" s="89" t="s">
         <v>197</v>
       </c>
-      <c r="M7" s="84"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
       <c r="P7" s="84"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="75"/>
-    </row>
-    <row r="8" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q7" s="85"/>
+      <c r="R7" s="85"/>
+      <c r="S7" s="84"/>
+      <c r="T7" s="106"/>
+      <c r="U7" s="75"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="65" t="s">
         <v>52</v>
       </c>
       <c r="B8" s="60"/>
       <c r="C8" s="40"/>
       <c r="D8" s="40"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="89" t="s">
+      <c r="E8" s="60"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="105" t="s">
+        <v>241</v>
+      </c>
+      <c r="I8" s="105" t="s">
+        <v>242</v>
+      </c>
+      <c r="J8" s="105" t="s">
+        <v>241</v>
+      </c>
+      <c r="K8" s="105" t="s">
+        <v>242</v>
+      </c>
+      <c r="L8" s="89" t="s">
         <v>192</v>
       </c>
-      <c r="J8" s="89" t="s">
+      <c r="M8" s="89" t="s">
         <v>193</v>
       </c>
-      <c r="K8" s="89" t="s">
+      <c r="N8" s="89" t="s">
         <v>194</v>
       </c>
-      <c r="L8" s="89" t="s">
+      <c r="O8" s="89" t="s">
         <v>195</v>
       </c>
-      <c r="M8" s="84"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
       <c r="P8" s="84"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="75"/>
-    </row>
-    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Q8" s="85"/>
+      <c r="R8" s="85"/>
+      <c r="S8" s="84"/>
+      <c r="T8" s="106"/>
+      <c r="U8" s="75"/>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="65" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="60"/>
       <c r="C9" s="40"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
       <c r="H9" s="84"/>
-      <c r="I9" s="89" t="s">
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="J9" s="89" t="s">
+      <c r="M9" s="89" t="s">
         <v>199</v>
       </c>
-      <c r="K9" s="89" t="s">
+      <c r="N9" s="89" t="s">
         <v>198</v>
       </c>
-      <c r="L9" s="89" t="s">
+      <c r="O9" s="89" t="s">
         <v>198</v>
       </c>
-      <c r="M9" s="84"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
       <c r="P9" s="84"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="75"/>
-    </row>
-    <row r="10" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="Q9" s="85"/>
+      <c r="R9" s="85"/>
+      <c r="S9" s="84"/>
+      <c r="T9" s="106"/>
+      <c r="U9" s="75"/>
+    </row>
+    <row r="10" spans="1:21" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="60"/>
       <c r="C10" s="40"/>
       <c r="D10" s="40"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
       <c r="H10" s="84"/>
-      <c r="I10" s="89" t="s">
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="89" t="s">
         <v>200</v>
       </c>
-      <c r="J10" s="89" t="s">
+      <c r="M10" s="89" t="s">
         <v>200</v>
       </c>
-      <c r="K10" s="89" t="s">
+      <c r="N10" s="89" t="s">
         <v>201</v>
       </c>
-      <c r="L10" s="89" t="s">
+      <c r="O10" s="89" t="s">
         <v>201</v>
       </c>
-      <c r="M10" s="84"/>
-      <c r="N10" s="85"/>
-      <c r="O10" s="85"/>
       <c r="P10" s="84"/>
-      <c r="Q10" s="106"/>
-      <c r="R10" s="75"/>
-    </row>
-    <row r="11" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q10" s="85"/>
+      <c r="R10" s="85"/>
+      <c r="S10" s="84"/>
+      <c r="T10" s="106"/>
+      <c r="U10" s="75"/>
+    </row>
+    <row r="11" spans="1:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="B11" s="100" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="101" t="s">
-        <v>143</v>
-      </c>
-      <c r="D11" s="101" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="87"/>
-      <c r="F11" s="87"/>
-      <c r="G11" s="87"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="100" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="101" t="s">
+        <v>244</v>
+      </c>
+      <c r="G11" s="101" t="s">
+        <v>245</v>
+      </c>
       <c r="H11" s="87"/>
       <c r="I11" s="87"/>
       <c r="J11" s="87"/>
       <c r="K11" s="87"/>
       <c r="L11" s="87"/>
       <c r="M11" s="87"/>
-      <c r="N11" s="88"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="104" t="s">
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="88"/>
+      <c r="R11" s="88"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="104" t="s">
         <v>146</v>
       </c>
-      <c r="R11" s="75"/>
-    </row>
-    <row r="12" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="U11" s="75"/>
+    </row>
+    <row r="12" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
         <v>149</v>
       </c>
@@ -2298,76 +2453,92 @@
       <c r="D12" s="73" t="s">
         <v>152</v>
       </c>
-      <c r="M12" s="48" t="s">
+      <c r="E12" s="73" t="s">
+        <v>150</v>
+      </c>
+      <c r="F12" s="73" t="s">
+        <v>151</v>
+      </c>
+      <c r="G12" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="P12" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="N12" s="48" t="s">
+      <c r="Q12" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="O12" s="48" t="s">
+      <c r="R12" s="48" t="s">
         <v>153</v>
       </c>
-      <c r="P12" s="48" t="s">
+      <c r="S12" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="T12" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="Q13"/>
-    </row>
-    <row r="14" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T13"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="38"/>
       <c r="B14" s="47"/>
-      <c r="I14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="J14" s="37" t="s">
-        <v>160</v>
-      </c>
-      <c r="K14" s="37" t="s">
-        <v>160</v>
-      </c>
+      <c r="E14" s="47"/>
       <c r="L14" s="37" t="s">
         <v>160</v>
       </c>
-      <c r="Q14"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="M14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="N14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="O14" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="T14"/>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="92" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="E18" s="92" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="93" t="s">
         <v>191</v>
       </c>
+      <c r="E19" s="93" t="s">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E4:H4" r:id="rId1" display="https://pmc.ncbi.nlm.nih.gov/articles/PMC3387822/" xr:uid="{EAAEB933-E6CB-401B-BC9C-DDF1BA2C4BAF}"/>
-    <hyperlink ref="E7:H7" r:id="rId2" display="1.61 (1.38, 1.89)" xr:uid="{087D63A8-8673-4FED-B4AA-78355EFD0EAC}"/>
-    <hyperlink ref="E2:H2" r:id="rId3" display="3.42(2.37, 4.94)" xr:uid="{65242B69-0DF5-4CFB-B061-87593AF2D7D6}"/>
-    <hyperlink ref="E6:F6" r:id="rId4" display="1.14(1.10, 1.18)" xr:uid="{0AC82558-76D8-4A46-86CD-5715FEFF04A8}"/>
-    <hyperlink ref="G6:H6" r:id="rId5" display="1.14(1.10, 1.18)" xr:uid="{357E3F28-1993-4C05-B534-54AE92750BFE}"/>
-    <hyperlink ref="I8:L8" r:id="rId6" display="1.22 (1.17, 1.28)" xr:uid="{C6FBFCCC-6B18-467F-8641-01ACD17463C9}"/>
-    <hyperlink ref="I7:L7" r:id="rId7" display="1.18 (1.06, 1.31)" xr:uid="{C5E12774-A930-4FA2-908D-F9616EB66494}"/>
-    <hyperlink ref="I9:L9" r:id="rId8" display="1.10 (1.03, 1.18)" xr:uid="{A3C6A6BA-ABC5-480C-92FC-62A49715B851}"/>
-    <hyperlink ref="I10:L10" r:id="rId9" display="1.12 (1.07, 1.18)" xr:uid="{BAE65CBC-6E4B-4AA4-B583-22AB3104651C}"/>
-    <hyperlink ref="I3:L3" r:id="rId10" display="https://pubmed.ncbi.nlm.nih.gov/26026348/" xr:uid="{255D8DE5-2107-481F-890F-EA2766EE6B49}"/>
-    <hyperlink ref="I6:L6" r:id="rId11" location="sec13" display="1.22(1.10, 1.36)" xr:uid="{D11D85F1-696C-46A5-9467-2367C9E3106E}"/>
-    <hyperlink ref="M6:O6" r:id="rId12" display="1.18 (1.10, 1.28)" xr:uid="{5F6D7853-A74B-4815-8147-2751460FADAD}"/>
-    <hyperlink ref="P6" r:id="rId13" xr:uid="{D15ADC47-A92A-4580-837C-5FFB47A655C8}"/>
-    <hyperlink ref="Q6" r:id="rId14" display="0.903(0.851, 0.952)" xr:uid="{9AE18721-A9FB-47DB-86F2-805C3DBFBB29}"/>
-    <hyperlink ref="I5:L5" r:id="rId15" display="1.01 (0.92, 1.12)" xr:uid="{B1375934-87C9-4618-A990-C5A10D987D42}"/>
-    <hyperlink ref="B2:D2" r:id="rId16" location="sec10" display="1.13(1.00, 1.26)" xr:uid="{02577497-1FFF-4721-BB88-67E7C8483FEC}"/>
-    <hyperlink ref="B6:D7" r:id="rId17" location="sec10" display="0.99 (0.95, 1.04)" xr:uid="{223F5910-7C9F-4125-92C2-315C39551190}"/>
-    <hyperlink ref="B11:D11" r:id="rId18" location="sec10" display="1.04 (1.01, 1.07)" xr:uid="{BF6EF940-63BA-4551-BF0D-43B13E59C027}"/>
-    <hyperlink ref="I4:L4" r:id="rId19" display="1.09 (1.02, 1.16)" xr:uid="{4C515288-CAF1-4FC9-92C6-22CC56393AA9}"/>
-    <hyperlink ref="Q11" r:id="rId20" display="0.967(0.937, 0.998)" xr:uid="{BA1C939E-1C5F-49DE-88F3-1DB70A5A2513}"/>
-    <hyperlink ref="Q3" r:id="rId21" location="full-view-affiliation-1" xr:uid="{D693F8E4-BF53-45A6-B723-FFEF11CFAC89}"/>
-    <hyperlink ref="Q6:R11" r:id="rId22" display="0.95(0.88, 1.02)" xr:uid="{04A2415D-1278-428E-A4B9-9E32892683B4}"/>
+    <hyperlink ref="H4:K4" r:id="rId1" display="https://pmc.ncbi.nlm.nih.gov/articles/PMC3387822/" xr:uid="{EAAEB933-E6CB-401B-BC9C-DDF1BA2C4BAF}"/>
+    <hyperlink ref="H7:K7" r:id="rId2" display="1.61 (1.38, 1.89)" xr:uid="{087D63A8-8673-4FED-B4AA-78355EFD0EAC}"/>
+    <hyperlink ref="H2:K2" r:id="rId3" display="3.42(2.37, 4.94)" xr:uid="{65242B69-0DF5-4CFB-B061-87593AF2D7D6}"/>
+    <hyperlink ref="H6:I6" r:id="rId4" display="1.14(1.10, 1.18)" xr:uid="{0AC82558-76D8-4A46-86CD-5715FEFF04A8}"/>
+    <hyperlink ref="J6:K6" r:id="rId5" display="1.14(1.10, 1.18)" xr:uid="{357E3F28-1993-4C05-B534-54AE92750BFE}"/>
+    <hyperlink ref="L8:O8" r:id="rId6" display="1.22 (1.17, 1.28)" xr:uid="{C6FBFCCC-6B18-467F-8641-01ACD17463C9}"/>
+    <hyperlink ref="L7:O7" r:id="rId7" display="1.18 (1.06, 1.31)" xr:uid="{C5E12774-A930-4FA2-908D-F9616EB66494}"/>
+    <hyperlink ref="L9:O9" r:id="rId8" display="1.10 (1.03, 1.18)" xr:uid="{A3C6A6BA-ABC5-480C-92FC-62A49715B851}"/>
+    <hyperlink ref="L10:O10" r:id="rId9" display="1.12 (1.07, 1.18)" xr:uid="{BAE65CBC-6E4B-4AA4-B583-22AB3104651C}"/>
+    <hyperlink ref="L3:O3" r:id="rId10" display="https://pubmed.ncbi.nlm.nih.gov/26026348/" xr:uid="{255D8DE5-2107-481F-890F-EA2766EE6B49}"/>
+    <hyperlink ref="L6:O6" r:id="rId11" location="sec13" display="1.22(1.10, 1.36)" xr:uid="{D11D85F1-696C-46A5-9467-2367C9E3106E}"/>
+    <hyperlink ref="P6:R6" r:id="rId12" display="1.18 (1.10, 1.28)" xr:uid="{5F6D7853-A74B-4815-8147-2751460FADAD}"/>
+    <hyperlink ref="S6" r:id="rId13" xr:uid="{D15ADC47-A92A-4580-837C-5FFB47A655C8}"/>
+    <hyperlink ref="T6" r:id="rId14" display="0.903(0.851, 0.952)" xr:uid="{9AE18721-A9FB-47DB-86F2-805C3DBFBB29}"/>
+    <hyperlink ref="L5:O5" r:id="rId15" display="1.01 (0.92, 1.12)" xr:uid="{B1375934-87C9-4618-A990-C5A10D987D42}"/>
+    <hyperlink ref="L4:O4" r:id="rId16" display="1.09 (1.02, 1.16)" xr:uid="{4C515288-CAF1-4FC9-92C6-22CC56393AA9}"/>
+    <hyperlink ref="T11" r:id="rId17" display="0.967(0.937, 0.998)" xr:uid="{BA1C939E-1C5F-49DE-88F3-1DB70A5A2513}"/>
+    <hyperlink ref="T3" r:id="rId18" location="full-view-affiliation-1" xr:uid="{D693F8E4-BF53-45A6-B723-FFEF11CFAC89}"/>
+    <hyperlink ref="T6:U11" r:id="rId19" display="0.95(0.88, 1.02)" xr:uid="{04A2415D-1278-428E-A4B9-9E32892683B4}"/>
+    <hyperlink ref="B2:G2" r:id="rId20" display="1.20 (1.06, 1.35)" xr:uid="{2E705ADD-D7A0-4860-96A0-2EC7C628742C}"/>
+    <hyperlink ref="B6:G7" r:id="rId21" display="1.05 (0.95, 1.16)" xr:uid="{3F031EC5-6061-4BAC-850A-6628A3F85932}"/>
+    <hyperlink ref="H8:K8" r:id="rId22" display="1.39 (1.28, 1.51)" xr:uid="{2D7B5991-1527-4127-8CE6-F423D1063C19}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
@@ -2378,9 +2549,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E34ADE-CF51-4185-BC0D-591DEA3B8782}">
   <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="W9" sqref="W9"/>
+      <selection pane="topRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2877,14 +3048,13 @@
     <hyperlink ref="I3:L3" r:id="rId16" display="https://pubmed.ncbi.nlm.nih.gov/26026348/" xr:uid="{DAF8F591-400B-442E-86AE-93BB8CB15CD8}"/>
     <hyperlink ref="I5:L5" r:id="rId17" display="1.01 (0.92, 1.12)" xr:uid="{B1514570-EBD5-4145-AC59-A8A3D814EC05}"/>
     <hyperlink ref="I4:L4" r:id="rId18" display="1.09 (1.02, 1.16)" xr:uid="{B2AD435A-7BF4-4BE7-9D09-ADEFA67CF3A2}"/>
-    <hyperlink ref="J11:L11" r:id="rId19" display="1.10 (1.06, 1.13)" xr:uid="{FB51944E-A5F0-47E9-AD12-FADF6B2EFD86}"/>
-    <hyperlink ref="Q3" r:id="rId20" location="full-view-affiliation-1" xr:uid="{0C6124C5-70A8-40F6-85E8-CB17A0954AAD}"/>
-    <hyperlink ref="Q6" r:id="rId21" display="0.903(0.851, 0.952)" xr:uid="{ACC8151D-4E96-4928-A2B4-DC7A70BC60F4}"/>
-    <hyperlink ref="Q11" r:id="rId22" display="0.967(0.937, 0.998)" xr:uid="{A959D47B-8580-4EBB-8F2A-1AF2629A3EC9}"/>
-    <hyperlink ref="Q6:R11" r:id="rId23" display="0.95(0.88, 1.02)" xr:uid="{713326FD-45B4-4FD7-B233-010BE5CA4134}"/>
+    <hyperlink ref="Q3" r:id="rId19" location="full-view-affiliation-1" xr:uid="{0C6124C5-70A8-40F6-85E8-CB17A0954AAD}"/>
+    <hyperlink ref="Q6" r:id="rId20" display="0.903(0.851, 0.952)" xr:uid="{ACC8151D-4E96-4928-A2B4-DC7A70BC60F4}"/>
+    <hyperlink ref="Q11" r:id="rId21" display="0.967(0.937, 0.998)" xr:uid="{A959D47B-8580-4EBB-8F2A-1AF2629A3EC9}"/>
+    <hyperlink ref="Q6:R11" r:id="rId22" display="0.95(0.88, 1.02)" xr:uid="{713326FD-45B4-4FD7-B233-010BE5CA4134}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId23"/>
 </worksheet>
 </file>
 
@@ -2893,10 +3063,10 @@
   <dimension ref="A1:AR20"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3418,7 +3588,9 @@
         <v>52</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="C8" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="D8" s="6" t="s">
         <v>44</v>
       </c>
@@ -3998,7 +4170,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>